<commit_message>
data updated on 2025-11-24 13:12:12.579262
</commit_message>
<xml_diff>
--- a/output/2025/scraped_data/National Health Fund 2025.xlsx
+++ b/output/2025/scraped_data/National Health Fund 2025.xlsx
@@ -2206,7 +2206,7 @@
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>Lobista</t>
+          <t>Gestor de intereses</t>
         </is>
       </c>
       <c r="M43" t="inlineStr">
@@ -21430,7 +21430,7 @@
       </c>
       <c r="L458" t="inlineStr">
         <is>
-          <t>Lobista</t>
+          <t>Gestor de intereses</t>
         </is>
       </c>
       <c r="M458" t="inlineStr">
@@ -21462,7 +21462,7 @@
       </c>
       <c r="L459" t="inlineStr">
         <is>
-          <t>Lobista</t>
+          <t>Gestor de intereses</t>
         </is>
       </c>
       <c r="M459" t="inlineStr">
@@ -21494,7 +21494,7 @@
       </c>
       <c r="L460" t="inlineStr">
         <is>
-          <t>Lobista</t>
+          <t>Gestor de intereses</t>
         </is>
       </c>
       <c r="M460" t="inlineStr">
@@ -56722,7 +56722,7 @@
       </c>
       <c r="L1178" t="inlineStr">
         <is>
-          <t>Lobista</t>
+          <t>Gestor de intereses</t>
         </is>
       </c>
       <c r="M1178" t="inlineStr"/>

</xml_diff>